<commit_message>
Fix <Fichier comptable> generation issue
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_virements_xlsx/état_des_virements_9_2022.xlsx
+++ b/download/generated situation/état_des_virements_xlsx/état_des_virements_9_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1010,9 +1010,44 @@
         <v>10200</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="B19" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C19" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D19" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E19" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F19" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G19" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="H19" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I19">
+        <v>272000</v>
+      </c>
+      <c r="J19">
+        <v>27900</v>
+      </c>
+      <c r="K19">
+        <v>244100</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K19"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>